<commit_message>
Get daily reddit data: Tue Dec  3 08:11:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C505"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3474 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1h5iguf</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long natural nails </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5iguf</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1h5idt6</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Yellow nails make me happy 🌻</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rms7tt4z9l4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1h5ib67</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in love </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ib67</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1h5i2dy</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>christmas nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5i2dy</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1h5hinp</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Candy cane dotticure ♥️</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f8ofspwyk4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1h5hhqm</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Hack for typing with long nails</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5hhqm/hack_for_typing_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1h5glyg</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>How to keep nails clean and healthy?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5glyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1h5fg9e</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Nail glue recommendations</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5fg9e/nail_glue_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1h5h9io</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkle and shine for the season! </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5h9io/sparkle_and_shine_for_the_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1h5g3d1</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Contact Dermatitis </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5g3d1/contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1h5gzt9</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic sparkles </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrodl3mlsk4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1h5ggi6</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Builder Gel progress 😍</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq9357bmmk4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1h5g489</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Lover Era</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh3foh2yik4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1h5fi1o</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Last month's ghost Pokemon nails!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5fi1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1h5fgah</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Icicle Nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku4f7we7ck4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1h5f7rz</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Glamnetic Caramel Apple</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5f7rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1h5eyfc</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ho ho ho! </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mx2q8v17k4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1h5ehtg</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Same of my favorite sets </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ehtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1h5ctry</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Professional gel x nails look like 💩</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ctry</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1h5dr47</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>blink-182 Nails!!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6201taskvj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1h5d5y6</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>So hard to get a good close up Mr. Devil 💅☃️🎄🎅</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/881xjz07qj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1h5d1ob</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>What shape do you think suits me?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hq7wdk2pj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1h5cmj4</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>I had my winter nails done yesterday.🥹😍❄️</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5cmj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1h5cf2q</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gemmed Cat Eye Polish </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5cf2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1h5cbzd</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>🩸</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxmq7svrij4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1h5byhc</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Practicing holiday art</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5byhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1h5b5kw</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you create BIAB nails that last? Tell me in detail please! </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5b5kw/how_do_you_create_biab_nails_that_last_tell_me_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1h5b3hw</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>KISS IMpress nails</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5b3hw/kiss_impress_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1h5ayqs</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>✨🎀 something simple 🎀✨</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bissm96y6j4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1h5auuf</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>OBSESSED with my holiday cateye</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5auuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1h5ag31</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Birthday set! Dip powder</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t77yz2ym2j4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1h5a844</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>too much growth for a fill in?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8djlipmr0j4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1h59zal</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>I really don't think the problem is nail prep but idk what else it could be :((</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h59zal/i_really_dont_think_the_problem_is_nail_prep_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1h59lnw</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Essential gift ideas for wife</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h59lnw/essential_gift_ideas_for_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1h59keu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st time for design nails </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkuc0nhgvi4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1h59dmw</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute simple Christmas nails </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq8zfw5yti4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1h5938x</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>🎄🎁❄️</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5938x</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1h59124</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Christmas nails ❄️ 🌲</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h59124</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1h58i5e</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Obsessed with green chrome!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5uf57e4ni4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1h581dw</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xeno4ptgji4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1h57i4f</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>That's a new one</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbe9p5hgfi4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1h56zze</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Why do they do this???</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h56zze</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1h571mt</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>First time trying press ons and I don’t think I can go back to regular polish!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dcypam1ci4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1h56v63</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>December nails 💎</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h56v63</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1h56mt1</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting Started With Nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h56mt1/getting_started_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1h56lly</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>My 3 month journey learning to use gel polish. It's not perfect yet, but it makes me happy.</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h56lly</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1h56776</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>my first Christmas nails!! :)</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h56776</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1h55qio</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I make them look better </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55qio</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1h55zgo</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>My Late Autumn Nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55zgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1h55gma</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Haute couture fashion moden - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55gma</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1h55m4n</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Doing Powder and Tips at Home for the First Time</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9iptdmn1i4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1h55d67</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My little sister wants a nail polish dryer--any recommendations </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h55d67/my_little_sister_wants_a_nail_polish_dryerany/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1h55c3d</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>🩷 Pink girly nails 🩷</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43ysjw2nzh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1h555la</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h555la</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1h54ixy</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Does this shape have a name?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l97wjdrpth4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1h54a6f</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for recommendations! </t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h54a6f/looking_for_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1h549kj</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Santa nails!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h549kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1h54lf3</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5op1wz7uh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1h54bb4</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>WICKED</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h54bb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1h53voz</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Rudolf Red Sparkles</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7z0zjck0ph4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1h53kf8</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mddk8iqmh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1h52x9x</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! What do I book to achieve this inspo pic from nailartist_kaori on instagram? </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyxzug54ih4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1h53794</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Christmas nails by me ❄️</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ciam5v3kh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1h5337q</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">birthday set (11/18) </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4l2s98ajh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1h52yck</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>first time doing nails!!! how did i do :)</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctvb32wbih4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1h52wot</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>White smudging?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk8agehzhh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1h52txa</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I get my nails done in their current state? </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h52txa</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1h52cfw</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My dip is cracking :( whyyyy    Gel came off thumb but it’s very cracked under gel on all fingers almost </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ebcn3rvdh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1h526mj</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My Silent Night set 🌙 ✨</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku0farkpch4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1h51r6e</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>IT’S TIIIIIIIIIIIIIIIIIIME ❤️💃🏻</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gju9okgn9h4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1h513g8</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Sharing my Turkey day nails sorry it is late</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/plcayajy4h4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1h50l9x</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flat nails? </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h50l9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1h50u28</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made it myself in gel, what do you think? </t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h50u28</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1h50rp9</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">l'Oreal Masked Affair in bright sunshine sold for a very short time in walgreens about 11 years ago </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxa0zn1o2h4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1h4zrmw</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>how to start charging my friend ?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h4zrmw/how_to_start_charging_my_friend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1h4miem</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>What is this white squeezed to make this 3d art 🥰💕</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajukuojb2d4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1h504r8</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Should I expect to pay for them to fix this?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h504r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1h503fk</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>color match?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h503fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1h4zjy9</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>first time getting my nails done…</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4zjy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1h4zg5n</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY Magnetic Nails - how did I do? </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lh19i4e3tg4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1h4z79b</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying long Acrylic nails 💅🏾 </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rukxml49rg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1h4ye7d</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>My friend made this💜💜</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4ye7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1h4ydz7</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>First time ever getting my nails done.. I LOVE THEM!!</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ib49e89lg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1h4y5x1</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">chat are these giving? </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4y5x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1h4xzqe</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rxt7vli9ig4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1h4wk4j</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Any tips on how to heal picked skin around finger tips? Can I get them done? Engagement Prep</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h4wk4j/any_tips_on_how_to_heal_picked_skin_around_finger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1h4v8ch</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>The name of the style where it looks like glitter is IN the mail?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h4v8ch/the_name_of_the_style_where_it_looks_like_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1h4wz6t</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>That reflective glitter tho🤩</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3heakcoeag4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1h4wo8c</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>They shine!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srngqe538g4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1h4wlm1</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>christmas nails!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4wlm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1h4vexk</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4vexk</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1h4vea3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Set I’ve done !!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4vea3</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1h4u9v2</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>After years without doing my nails...</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz362cjtmf4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1h4u9iy</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My daughter’s nails how did the tech do? </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4u9iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1h4u6i0</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Peach 🍑</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idseqrgvlf4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1h4tdt2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic to Biab? </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h4tdt2/acrylic_to_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1h4sukx</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>I love flowers 🌸💅🏻</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbom501h7f4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1h4skz4</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nail lady do good? </t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhja45s84f4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1h4r41a</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried something different. </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4r41a</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1h4qzhl</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>🎀✨</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4qzhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1h5ilwp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Poisonberry 🫐</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ilwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1h5ifnz</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>I feel like this magnetic holo is slept on</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/38d5rcknal4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1h5ibyp</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>What do you use to file your nails?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5ibyp/what_do_you_use_to_file_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1h5hmkj</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>ISO a stamping plate with this heart pattern!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5hmkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1h5hdh6</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Gift Suggestions from a desperate husband.</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5hdh6/gift_suggestions_from_a_desperate_husband/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1h5haon</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>KBShimmer</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5haon/kbshimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1h5gxip</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Need advices !</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5gxip/need_advices/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1h5gqzv</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I never do seasonally appropriate nail art but there's a first time for everything! 🎄(contains products received as PR) </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5gqzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1h5g245</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fields Of Lavender is beyond gorgeous </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5g245</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1h5g05o</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Brands QDTC &amp; base coat… Affordable </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5g05o/best_brands_qdtc_base_coat_affordable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1h5fv50</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting over it </t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5fv50</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1h5fdeo</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie - at sea level </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5fdeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1h5evka</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>{PR} OOOP - Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5evka</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1h5esdo</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Had to restrain myself a bit—but I’m very pleased overall with my little BF haul 💕</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5esdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1h5ejyb</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Getting Festive</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ejyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1h5e2wp</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Welp, I did it again crew...</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cgmnksnyj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1h5dmrk</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Lyn B “Cat’s Paw” is so delicate and peaceful, I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5dmrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1h5dknl</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Feeling festive</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5dknl</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1h5d9hk</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas mani time! </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5d9hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1h5d5ns</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Feeling wintery ❄️</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5d5ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1h5clxn</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Inspired by the beetle post</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5clxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1h5c6c9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Looking for similar colour of nail polish</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ac5u5dbhj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1h5c3hl</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>My lil emo Christmas mani</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5c3hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1h5bsau</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>What are your favorite swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5bsau/what_are_your_favorite_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1h5bovl</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Happy Little Accident</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5bovl</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1h5b6wp</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Total drying time?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5b6wp/total_drying_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1h5b23m</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Zoya BF Sale Issues?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a391wo9o7j4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1h5axhd</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨🎀 something simple 🎀✨ </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7kplp1fn6j4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1h5awvu</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Gunmetal Accident</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g73c4wyi6j4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1h5aikt</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Your Heart's A Black Hole</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6xgt70o73j4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1h59i2g</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Unfulfilled Mooncat Orders</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h59i2g/unfulfilled_mooncat_orders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1h599e2</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Why is taking nail photos in natural light always such a workout??</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h599e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1h58yzk</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Theme: Baby Metal</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h58yzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1h58qpv</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Get a Helmer, they said</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h58qpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1h58dv5</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Anyone remember the name of this polish from Live Love Polish(now Mooncat)?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h58dv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1h57tm7</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Mods deleted original post. Posting again. Trying layering out for winter mani</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h57tm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1h57r93</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Olive &amp; June ruined my nails in one manicure. So, which companies are better than them?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b6fqdrchi4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1h579y2</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you ever just find a perfect patch of sunlight to admire your nails in </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ici9k45rdi4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1h56btt</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Inspired Wicked Manicure</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clj76oft6i4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1h566wo</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Has anyone tried the jelly polishes from Emily De Molly?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h566wo/has_anyone_tried_the_jelly_polishes_from_emily_de/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1h55oz1</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Extensions: Builder Gel + Forms vs Gel Tips?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h55oz1/extensions_builder_gel_forms_vs_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1h55mn5</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer statement</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55mn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1h55iki</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>THE SHIFTIEST! Cupcake polish cloud 9</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wnxxztks0i4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1h5599n</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Please help me</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5599n</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1h54sks</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Existential Crisis and Menchie the Cat</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h54sks</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1h545yw</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Ok, y'all influenced me! Ordered 8 mini bottles of Daisy Chain Polish! :) Can't wait to try them out!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h545yw</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1h543tr</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Holo Taco Cloud Nine</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blu21ihoqh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1h53zn1</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Told my partner I “had a vision”</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h53zn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1h5291z</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnetic Recommendations </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5291z/magnetic_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1h52111</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Black Friday haul🖤🩷</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h52111</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1h51lbl</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>I was thinking Christmas but I also feel it gives glam John Deer vibes. Jean Deere.</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diuc0wpi8h4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1h51jpk</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Starting December off right!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h51jpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1h51bmb</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Holiday hair is bananas!</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h51bmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1h50xm6</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Light the Way by EDM</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h50xm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1h50s7h</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">L'oreal Masked Affair in bright sunshine sold for a very short time in walgreens about 11 years ago </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w4zrw5s2h4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1h50izp</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Baeocystin 🍄</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9cetl45b0h4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1h50gp3</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to get myself in the Christmas spirit. </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h50gp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1h5081a</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am doing my best with streaky mail polish </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyhuwlcqyg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1h5002d</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Sample sized bottles?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5002d/sample_sized_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1h4zo3y</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love all of you nails queen 👸🏻 </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4zo3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1h4zjxq</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">swipe for nakie pics 😜 </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4zjxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1h4z85l</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Mooncat Jewel Beetle</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8vrkdtfrg4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1h4z31g</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Anyone know where I can buy nail stickers and charms like these? I have been finding ones that are similar, but they are not pastel colored/waaaay too big.</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuks1mfeqg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1h4yn77</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>had to cut my nails short to learn guitar but i think they still look nice :)</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzsoopx6ng4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1h4y87o</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>🎄holiday colors</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo9oa7m4kg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1h4xx30</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Ravishing Gown 💜✨</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4xx30</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1h4xrjn</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My First Thermal Nail Polish! </t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4xrjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1h4wyns</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Etsy $5 off $25 today</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4wyns/etsy_5_off_25_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1h4wu50</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Fall skittle (even though it’s snowing)</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecd7done9g4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1h4vdqq</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Essie Sand in my suit</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4vdqq/essie_sand_in_my_suit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1h4vdm0</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>🍄🎮Mario Skittle PART II⭐️🍄</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4vdm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1h4uov8</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>How do you get rid of nail polish?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4uov8/how_do_you_get_rid_of_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1h4shgv</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4shgv/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1h4bu0z</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>ILNP BF order</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4bu0z/ilnp_bf_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1h4ehqa</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dupe for lidl's "cien winter sparkles 139" </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4ehqa/dupe_for_lidls_cien_winter_sparkles_139/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1h4gonk</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your fave ILNP polishes </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4gonk/your_fave_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1h5iheb</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long natural nails </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5iheb</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1h5e6sw</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Ame is set!!!!! 😍</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0prnd6kozj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1h5dt8q</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Anyone else do their nails to match the weather lol</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bopwp935wj4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1h5ajg3</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>first ever attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tqvht9e3j4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1h59tcu</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Beautiful nails from Nayelis</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktjmpbhhxi4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1h594yu</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still sorta new to gel, how are my nails? Advice </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h594yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1h59165</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Potential?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h59165</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1h57yrq</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Chrome nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h57yrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1h56r82</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blueberry nails with blue flowers painted by me! 🫐💙 Inspired by pics on Pinterest :) </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cyo9unw9i4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1h56dnu</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Christmas press on design </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9le3dku57i4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1h55mf6</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just cutes! a pink color is always need it </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55mf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1h55jo4</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>My first lace nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qckm88r51i4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1h55i6f</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Haute couture fashion moden - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55i6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1h55bok</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>🩷 Pink girly nails 🩷</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37o30s0kzh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1h55aup</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>help are my nails ugly</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h55aup</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1h559k9</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Discreet and beautiful😍</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oucuzz04zh4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1h54dbs</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Choose my Winter Nails </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h54dbs/choose_my_winter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1h5489k</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Wicked Set</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5489k</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1h53yut</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Which of these can I show off around with confidence?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h53yut</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1h53fjk</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Cookies and Creme🍪🥛🍪</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/drrea0dolh4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1h53f1b</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Snakeskin Dualform</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jqj5mv5llh4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1h50djc</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Burberry ❤️</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bzdwe8uzg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1h4yzhu</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>icicle nails🥶</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pob3zqyopg4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1h4vkib</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still practicing, but thought these little Christmas trees were cute </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gnft60tyf4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1h4vive</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Chromatic nails!!✨</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3oo1pq3dyf4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1h4u70h</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>I love this design</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y2qaiy0mf4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1h4sgj2</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>New stuff ✨</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h4sgj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1h35brp</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One week retention-original art </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu3sp09d3z3e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec  4 08:11:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C505"/>
+  <dimension ref="A1:C695"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9018,6 +9018,3236 @@
         </is>
       </c>
     </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1h6b24u</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Noooooooo! And owwwwww! </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh00t31ngs4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1h69v2f</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlr8s2ef1s4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1h69nl0</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Junk nail set!!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h69nl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1h69h6e</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Educate me please!!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h69h6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1h68l2h</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got these done…not my favourite set…. They are ok….its not quite what I asked for. </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h68l2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1h69cvg</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h69cvg/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1h696xl</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Am I the odd one out?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67e1jumvtr4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1h694pk</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Bumblebee nails</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h694pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1h68od1</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Christmas Nails❤️💚</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h68od1</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1h687kb</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail tech always comes in clutch with cute critters! </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bju664xpjr4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1h67oi2</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND Gel Order came today! </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsc7q4hber4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1h67hum</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art :’)</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41pjiy9icr4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1h65lb0</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Can I put builder gel (cured) under press-ons?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h65lb0/can_i_put_builder_gel_cured_under_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1h66b50</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Longer nails = fewer chips?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h66b50/longer_nails_fewer_chips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1h6766b</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Winter Nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6766b</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1h673s4</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Kirby :D</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h673s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1h66z77</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>How are you guys typing!?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h66z77/how_are_you_guys_typing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1h66b8x</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel pedi I did on myself &amp; my first time doing a French tip </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7fnud1e1r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1h6678k</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>First time using press on nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx3eq74e0r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1h65upk</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail tech always spot on!!! </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m962oag9xq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1h65j5p</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I’m obsessed! Still can’t believe I got this on the 1st try 💖🖤</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h65j5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1h65gtf</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not sure if I love or hate these </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eknpmtzqtq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1h64tve</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>‘Tis the season ✨</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7u9cm64oq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1h64tuf</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>How much do y'all tip?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h64tuf/how_much_do_yall_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1h63izo</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbnda5hzcq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1h63eem</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>My petals atm🎄✨️</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znti8jivbq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1h630ru</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Dip w/out UV</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h630ru/dip_wout_uv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1h628ex</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Since it's December I thought I'd get into the Christmas Spirit!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8r2smuh2q4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1h61zip</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>My first year doing Christmas/Winter nails!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h61zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1h61kp3</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>any gel polish recommendations that match this jelly pink nude color?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h61kp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1h614mc</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>First time getting cat eye nails and I'm in love</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h614mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1h606km</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My nail artist is so talented 😍 I can’t stop looking at them</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loinu9ekmp4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1h5zzum</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Nail Strengthener Polish Coated On Press-On Nails?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5zzum/nail_strengthener_polish_coated_on_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1h5zwsb</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Problems with NKY1 glue</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5zwsb/problems_with_nky1_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1h5zwyz</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP combo </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5zwyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1h5yenq</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Powder manicure crumbling after 3 days- advice?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5yenq/powder_manicure_crumbling_after_3_days_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1h5z7gi</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5z7gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1h5yz22</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>The nurse matched Band-Aid to my nail polish</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il2u7mhndp4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1h5yh25</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Green spot at cuticle ?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tma9brzz9p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1h5ykxx</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat yellowing </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5ykxx/top_coat_yellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1h5x0gz</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>What nail shape could I do?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5x0gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1h5x75q</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kourtney Barker inspired nails 🎸 (trying this again w/o the cursed pose) </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5x75q</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1h5xik6</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Christmas nail art</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcp4h92w2p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1h5xijf</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I tried a thing</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ya1g5vwv2p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1h5xegf</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I got my nails done today 💕 Christmas green 💚</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5xegf</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1h5wrkv</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>What OPI color could this be?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge3bghqgxo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1h5wlb1</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Why do air bubbles form in these specific spots about half an hour after I finish my nails?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5wlb1/why_do_air_bubbles_form_in_these_specific_spots/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1h5vgv2</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do nail techs do this? </t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wx8ebs2aoo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1h5vqff</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5vqff</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1h5vmzd</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>I am IN LOVE with this new nail polish</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5vmzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1h5vme5</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>First set I made with press ons..constructive criticism?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6xgv6rdpo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1h5vdpg</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommended nail shape for my hands? </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5vdpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1h5ur11</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone have onycholysis (nail bed separating) occasionally? </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5ur11/anyone_have_onycholysis_nail_bed_separating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1h5uwsi</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd Jinx Nail Finished 🫶🏼😫 Grown up Powder (Arcane) </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjqjhy78ko4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1h5uusn</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Holidays! </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7jlig72sjo4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1h5ulfh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Wreath and Tree </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ulfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1h5ug8w</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>French Tip Question</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ug8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1h5u6a5</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am a Trans Woman who has decided to start doing my nails, this is the Late Autumn Set </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cnbj85sjeo4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1h5u5jb</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish won’t dry. No matter what. </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pqnhtyleo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1h5u2ci</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Nails for me X2</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8h5b2jydo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1h5tzxm</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Christmas nails 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdjndy4gdo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1h5tli3</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never in my life </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kepvj3rkao4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1h5sy0u</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>👸 Beauty and the Beast Nails 👸</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eb990jrr5o4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1h5rjfm</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>How do y'all do it??</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5rjfm/how_do_yall_do_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1h5rkuf</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>How do I wash my hair with acrylic nails</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5rkuf/how_do_i_wash_my_hair_with_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1h5rqa8</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>December set! 🫶🏻❤️💚</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5rqa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1h5rnnr</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Holographic claws</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t7zkc437wn4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1h5rhvc</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h35ncexun4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1h5r4ne</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Feeling cozy</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5r4ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1h5r063</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>love sparkles (new nails)</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5r063</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1h5pqnw</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>how do i fix these🥲</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5pqnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1h5n2i2</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Nail damage after removing gel</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5n2i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1h5n08l</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chat it’s so over </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wizy0okkum4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1h5jzak</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BIAB or gel ? </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwvcr0apvl4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1h5jsaa</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Polygel nails bending??</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqykaap3tl4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1h5qo77</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>At home gel help - what am I doing wrong? Lasts 2 days and is still tacky after application</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5qo77/at_home_gel_help_what_am_i_doing_wrong_lasts_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1h5pwqu</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>What do you think about those pearl-like pedicure?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5pwqu/what_do_you_think_about_those_pearllike_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1h5pu4v</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Desperately need a manicure but need advice </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5pu4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1h5poha</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>My nail artist did the most amazing Christmas set 🎄</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er8xbhg3hn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1h5pltc</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>How is this for a beginner</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oifsp94jgn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1h5pg5w</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>3d printed organization</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5nofd27fn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1h5p8rq</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Pink/blue</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9anu2cudn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1h5oukb</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Hold your nail techs tight ❤️</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5oukb</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1h5oug6</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">L.A COLOR Mermaid Mist </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5oug6</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1h5o5p9</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>My Christmas nails. With pics this time 😂</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5o5p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1h5o4mo</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails. </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5o4mo/my_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1h5nmpn</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>December mani ❄️</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5nmpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1h5n2in</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Nail tech overfilled my nails taking off my first acrylics ever - product/treatment tips?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5n2in/nail_tech_overfilled_my_nails_taking_off_my_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1h5mgsu</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Advice for natural nails</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5mgsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1h5m1up</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Holiday vibes 🎉🎊🎁 🎄</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5m1up</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1h5lu9j</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h5lu9j/first_time_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1h5l6f1</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6gykcl0bm4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1h5kgwc</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>3D nail art 💅🏻💫</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fswi4zy42m4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1h5jf2a</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Christmas Vibes</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3jr9us1ol4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1h69n7p</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Frosted ice nail polish</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h69n7p/frosted_ice_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1h69d1c</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Storage? </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h69d1c/storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1h690tb</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Snake Charmer</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h690tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1h690hx</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Canadians - where are you getting your magnets?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h690hx/canadians_where_are_you_getting_your_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1h688tr</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>My first successful stamping!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h688tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1h67xky</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>If your collection could only consist of 3 polishes from 1 brand, what would they be?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h67xky/if_your_collection_could_only_consist_of_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1h6774e</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>LynB, I love you</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6774e</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1h674ti</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Dupe of this Ad (Not the Actual Polish)</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0vzr9tz8r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1h66wc4</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Have your nails done</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4tr4ziq6r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1h65z81</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>indie christmas collections?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h65z81/indie_christmas_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1h65mpv</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Can I put builder gel (cured) under press-ons to prevent getting greenies?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h65mpv/can_i_put_builder_gel_cured_under_pressons_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1h658bn</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>I need to try one of these NOW!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/047ye2bmrq4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1h64px6</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my favorites I’ve done in a while! </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h64px6</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1h63n67</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Are there any places that do birthday deals for polishes??</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h63n67/are_there_any_places_that_do_birthday_deals_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1h63me2</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>🍋👑 Princess Lolly 👑🍋</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h63me2</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1h62qbs</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Mooncat palette</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h62qbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1h62g7t</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>WOW I can’t believe how much longer my mail beds have gotten!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h62g7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1h62g08</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>I was walking home drunk and couldn't stop starring at my xmas themed nails🙈</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h62g08</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1h61izl</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe requests </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h61izl/dupe_requests/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1h61d5x</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>did a nail portraiture in the grand manner style for art history class</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h61d5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1h60op0</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a nude barbie-hand palate cleanser before all the holiday glitter! </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvb7kedgqp4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1h609ql</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Pretty Chrome Skittle</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9hxvu1s7np4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1h603pb</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>hi. 💕💜</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmc8i59zlp4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1h5zfom</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your danish cookie/sewing box lid, my velvet setup </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9v5f5z3hp4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1h5yzbg</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry shiftmas to me! </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5yzbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1h5ynfd</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Am I crazy? Another cirque thread</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ynfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1h5ylvm</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Unhinged LA Colors Splurge</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ylvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1h5xuc0</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Top coat yellowing</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5xuc0/top_coat_yellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1h5xlez</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Zoya and ILNP Comparison</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5xlez/zoya_and_ilnp_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1h5xgty</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5xgty</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1h5xfly</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Broke my nails ripping off my Gel X :(</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kd5tvm92p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1h5wufn</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Got so distracted in the car</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5wufn</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1h5wmlf</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>‘Tis the season 🎁</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb36iw9jwo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1h5whrw</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Finally gota horseshoe magnet ✨</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5whrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1h5wc6k</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>It's the gingerbread man(i)!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5wc6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1h5vlak</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UPDATE on "Am I allowed to be dissapointed?" (Ard As Nails swatch inconsistency issue) </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/s/dEqogDSznu</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1h5vkcs</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Obsessed with ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc6xp92zoo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1h5vjng</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>This week's mani!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5vjng</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1h5v7um</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matched my Kindle </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjpwkkmgmo4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1h5uv5y</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try with velvet effect </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/07mp4f0wjo4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1h5upkh</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Anyone else have onycholysis (nail bed separating) occasionally?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5upkh/anyone_else_have_onycholysis_nail_bed_separating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1h5uhro</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Looking for help with a dupe</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojarg9j4ho4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1h5topi</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>mooncat haul skittles🌙</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5topi</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1h5tam8</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Blood Moon</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5tam8</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1h5t254</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails peeling after removing polish </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usvwfnml6o4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1h5srno</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Did my cousin's nails the other day</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5srno</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1h5sdq0</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Ethereal-Ether Dragon</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5sdq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1h5s8oy</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>How do you get used to having something on your nails?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5s8oy/how_do_you_get_used_to_having_something_on_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1h5s7di</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>first time Holo Taco buyer and I am stunned</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5s7di</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1h5s3nc</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minty Petals for a Narscissist </t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5s3nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1h5rzh7</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>My husband-made polish advent</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7dlujenyn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1h5rudr</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>A sacrifice was made</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5rudr</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1h5rhjo</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Is anyone else’s Cirque package stuck at the post office?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eulsj5fvun4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1h5qxzi</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Immortal Jellyfish 🪼</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5qxzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1h5q9iu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Chawkulit's 50% off BF Sale </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5q9iu/pink_chawkulits_50_off_bf_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1h5phi9</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Officially Christmas Nails Season</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5phi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1h5otl4</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t xml:space="preserve">L.A color Mermaid Mist </t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5otl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1h5oewp</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Essie Sand in my suit</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5oewp</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1h5nert</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Color Theory is Crazy</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5nert</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1h5n7uk</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>just a little cow print 🐮</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5n7uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1h4topl</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Methacrylate Allergy Question</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h4topl/methacrylate_allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1h591c8</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>KBShimmer reformulation not listed on website</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h591c8/kbshimmer_reformulation_not_listed_on_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1h596km</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Potential?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h596km</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1h5aedh</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Gray and shimmery combo for this season’s first snow</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5aedh</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1h5fujh</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Paddie Nails is a Scam</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5fujh</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1h5j01a</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Dam reflectives are one of the best out there!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5j01a</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1h6a6cx</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Green and gold festive nails</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yg59cqo95s4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1h69act</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">festive holiday nails by me! </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh66276xur4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1h6941x</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Cathedral motifs</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6941x</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1h67muj</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Today's app 😊</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx40rd1vdr4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1h67el4</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Bright pink🩷</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz9s0hymbr4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1h66xot</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>December Birthday nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ndmdbv27r4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1h66wt7</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>I changed the bows 😭😂 it’s giving classy Christmas ✨🎄</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h66wt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1h66bo3</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Holiday Nails - Im obsessed 😍 What do you think?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9d7pg3i1r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1h65upc</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thanksgiving nails I (43m) did for my daughter (13f) last week. </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h65upc</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1h65kgr</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Still can’t believe I got this on the 1st try, I’m obsessed 💖🖤</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h65kgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1h64jb9</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Trying, and admittedly failing, at trying my hand at sculpting and painting nail details. Everyone makes it look so easy but my goodness....</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h64jb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1h608eg</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These were fun to do.. </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gge87diump4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1h5z83p</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Arcane nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/np1yce1jfp4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1h5xs52</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Nails and purse ❤️✨</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl4582cv4p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1h5xcbj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I tried a thing</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo9ctvjl1p4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1h5wd7g</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Inspired by winter ❄️🏔</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5wd7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1h5w0pk</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Bday nails</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5w0pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1h5w05e</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Help me decide my next set!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h5w05e/help_me_decide_my_next_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1h5ux7d</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd Jinx Nail Finished 🫶🏼😫 Grown up Powder (Arcane) </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5ux7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1h5tqct</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Y2K nails </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxul9nuhbo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1h5t8gi</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>flirty christmas nails🎄✨️</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ogblh6y7o4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1h5sye7</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>👸 Beauty and the Beast Nails 👸</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y2tesqu5o4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1h5sdrb</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Sagittarius freestyle ✨💙</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5sdrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1h5s55u</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Fun stuff this week ✨</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5s55u</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1h5rx96</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wicked! green is good for this season </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gv32u618xn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1h5rtpv</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first set of Xmas nails for this year </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xnjirjgxn4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1h5rcxl</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter inspired nails set </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5rcxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1h5q6z0</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Just in time for Xmas</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxxgjoo0ln4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1h5n9fz</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>first set ive ever done on myself</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h5n9fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1h5km4d</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Butterflyyy</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yu2w3m14m4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec  5 08:12:04 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C695"/>
+  <dimension ref="A1:C892"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12248,6 +12248,3355 @@
         </is>
       </c>
     </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1h74cwe</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What are your best tips for trimming the toenails? I'm an endependent blind woman who was taught a lot about a lot, but not this lol.</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h74cwe/what_are_your_best_tips_for_trimming_the_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1h73kcr</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>New season, new set</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu00s4s4dz4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1h737if</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Nails </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lvebqyr8z4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1h72qht</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Any advice?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h72qht/any_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1h6zhvg</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>it's my first time to make press-ons 🥹! Inspired by wicked colors but used a white base 🪄🪄🪄</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klrpfzfi6y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1h6yy2f</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkitxe3e2y4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1h6yl3p</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Christmas Set</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t4qhq6azx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1h72hrk</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>What vibe do these give?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h72hrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1h72gic</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Square or Almond? </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h72gic</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1h72ebf</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>2nd Timer</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53lo6pqezy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1h727en</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>matte baby blue 🩵</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pg4xu18xy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1h71zaz</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying something new, not sure how I feel about it. Input? </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri968sfxuy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1h71vwr</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did you get rid of your nails peeling? I’m at my wits end! </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h71vwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1h71qo1</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>the most perfect color 😘</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmomzfigsy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1h71qcz</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/websih8dsy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1h70l98</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Cat eye black nails 🖤</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rj8l9k9hy4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1h701wj</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Would you wear your sign?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83leqzs9cy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1h6zuk6</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Gingerbread contest press ons. How did I do?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6zuk6/gingerbread_contest_press_ons_how_did_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1h6zmie</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>How long do you acrylic nails last without infill?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc6ds76c8y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1h6z79o</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do these scream press ons? </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6z79o</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1h6z20z</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>What extensions can I get for short bitten nails?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6z20z/what_extensions_can_i_get_for_short_bitten_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1h6xdfq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld9zj6snox4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1h6x2do</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas cat eye nails </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ect3tz1mx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1h6wt20</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Do my nails look healthy?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm56fj8xjx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1h6wl2n</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>My first set ever ✨ Done in Bangkok</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6wl2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1h6w8id</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Christmas nails done! What do you think?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6w8id</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1h6vy32</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>❤️🍭❄️💙</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vy32</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1h6vms8</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked color change </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vms8</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1h6vms6</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Christmas manicures</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vms6</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1h6vjno</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Hello red mani magic</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vjno</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1h6urr0</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>How can I take care of this mess I made?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgl3ue0g3x4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1h6u5pq</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does BIAB need to be removed and then applied if you’re getting a new colour put on? </t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6u5pq/does_biab_need_to_be_removed_and_then_applied_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1h6tzmg</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the best gel x tutorial you’ve found? </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6tzmg/what_is_the_best_gel_x_tutorial_youve_found/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1h6tkl2</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Shock reaction to Builder Gel… HELP!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6tkl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1h6tp38</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tomorrow is my graduation 🎓 </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6tp38</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1h6tnxx</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>christmas set 😭</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6tnxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1h6tmof</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Tangled Cat Eye Nails ✨</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6tmof</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1h6tklx</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>i am self taught, what do you think?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6tklx</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1h6tc4j</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done! </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mubrrbf6sw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1h6sowm</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Is gel allergy possible with fully cured nail wraps?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6sowm/is_gel_allergy_possible_with_fully_cured_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1h6t0qo</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Decided to try cat eye nails for the first time and I am obsessed!!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6t0qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1h6szgq</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>My new Christmas nails 💅</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6szgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1h6su8i</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Christmas set that I did yesterday to get festive!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6su8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1h6sh0w</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>So realistic it even gave my techs the creeps! (Spider warning)</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6sh0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1h6rcrc</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>My Christmas nails 🎄🎀</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkoin9vvdw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1h6r6co</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I need help with ideas</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6r6co/i_need_help_with_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1h6qp3d</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First time getting a manicure</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o68es959w4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1h6qeu7</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with red for my Christmas weekend holiday! </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6qeu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1h6pslz</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>I need to take outside pics more often. The sun is the best lighting lol</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgjboqdk2w4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1h6po9k</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Best Friend is Going to Japan for 3 Weeks. I sent her with $300 USD…what should she get for me?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6po9k/best_friend_is_going_to_japan_for_3_weeks_i_sent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1h6pmta</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time trying a frenchie </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/raae0rde1w4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1h6p6md</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Did My Nails at Home for the First Time</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6p6md</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1h6p1ha</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Do not buy from Ersa nails! They’re dropshippers masquerading as a small business!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6p1ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1h6oxde</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lisa Frank inspired nails! </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oust9qqawv4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1h6na5d</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Is there any way to blend gel x nails after application?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgg28hgnkv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1h6orhv</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>my nailtechs christmas magic ✨🎄❤️</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lr6yee5vv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1h6onwj</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tools to help with consistent nail shape? </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6onwj/any_tools_to_help_with_consistent_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1h6omog</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Chrome Polka dot 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqzwtza6uv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1h6oba8</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good nail salon in DMV area, germantown preferably </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o45e9cxrv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1h6o9s9</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This gal has an awful cold but managed to put on a base coat yesterday (does that count as unpolished?) </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o0fq5vlrv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1h6nngf</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Do my nails need a break?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6nngf</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1h6nl0v</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Christmas nails. 🌲☃️❄️</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0qvx9btmv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1h6mqkl</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>1st attempt at a candy cane</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6mqkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1h6mrog</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Classic black frenchies 😍</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6mrog</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1h6mltv</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what to do in this situation </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9wwwuuufv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1h6m70x</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Guys I need some advice pls</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6m70x/guys_i_need_some_advice_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1h6m6r7</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Do my nails have potential?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sjertdzcv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1h6m5y6</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Made my first press on nail set! Any areas for improvement?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/106qnt8ocv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1h6m0m4</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing lasts more than 16 days- help! </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6m0m4/nothing_lasts_more_than_16_days_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1h6lxuf</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Happy Holidays! 💚</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6lxuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1h6lrre</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Goldfinger press on?!?!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlpjb0c4av4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1h6kxgm</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with my friend who's also a nail tech </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6kxgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1h6kx2s</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Glistening Gale 🌬️</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6kx2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1h6hy0v</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Warped nails?? Please help</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6hy0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1h6kpxh</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How often can I apply this? Trying a few things while my nails are growing out stronger </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmwz4vyq2v4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1h6kdo2</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Does classic French suit me?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/995rj1ba0v4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1h6jes3</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Experiment using color plus top coat gel to create a jelly color</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/qWyOItE.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1h6bjno</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nail hardener/acrylic</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/875h8p6ans4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1h6bt5o</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>(Possible) contact Dermititis for specific colors?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6bt5o/possible_contact_dermititis_for_specific_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1h6j997</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>What to stick press on nails on with?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vencurp9su4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1h6j8a2</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>French neons💙💜🩷🧡💚</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wia9osz1su4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1h6hiqv</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Guyssss 😭 my nails are stained yellow after I used a red glitter nail polish...2 coats of it</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6hiqv/guyssss_my_nails_are_stained_yellow_after_i_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1h6ghdg</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Gingerbread inspired nails.</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psgx5ef97u4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1h6gc3g</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I shape these? I’m so lost. </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6gc3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1h6iob1</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My previous set for thanksgiving and my current set for Christmas </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6iob1</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1h6ijqq</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Teabag Trick</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6ijqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1h6irmp</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Peeling gel</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6irmp/peeling_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1h6inm1</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Christmas Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aihgic1xnu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1h6ihw1</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>🍀</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8ndb7crmu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1h6i0w1</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>ice princess nails ☆ still learning how to apply gel x on myself as a press on girly.</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6i0w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1h6hk9x</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guysss please help me yall my nails are stained yellow after I used a dark red nail polish...2 coats of it for 3-4 days </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h6hk9x/guysss_please_help_me_yall_my_nails_are_stained/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1h6grkl</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Should I trim the rest?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6grkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1h6ftbc</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>First Christmas nails for the month</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dqlm45l1u4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1h6fmqb</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Can you tell Purple is my fave? 💜 💅</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrz450n00u4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1h6fhrf</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">too big? </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6fhrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1h6fdey</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Winter</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ecpmq74oxt4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1h6f0b3</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">By me, on me. </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iob2u154ut4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1h6epn8</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>I did some sparkly blue gel nails for snow season</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n1gn364rt4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1h6ec3g</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>New Set - Coraline</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npum97y2nt4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1h6dicv</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6dicv</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1h71io5</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Omg my first mooncat order arrived! </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkaw7zh7qy4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1h710d4</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Talking about how light interacts with matter in class, so of course I needed to break out the flash-reactive polish.</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h710d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1h70c15</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Accidental Jinx mani. (Side note, I feel like Jinx would go nuts for a multichrome) </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pw8clveuey4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1h6zurv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>First Christmas mani of the year!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3snv4leay4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1h6zn5k</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Tricked Out &amp; Somebody's Fool</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35sa39qf8y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1h6zlez</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Singing the praises of Light Elegance</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jjlg9928y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1h6zj19</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I guess I’m a swatch girlie now </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/deepuj2g7y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1h6yzyh</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Matte topcoat</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6yzyh/matte_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1h6yam3</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Pigment of My Imagination by Sassy Sauce Polish is pure magic! </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6yam3</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1h6xg75</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Christmas </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6xg75</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1h6x6h2</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>mooncat sale purchases! swatch skittle :D</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6x6h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1h6x0hk</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Snow Princess vibes</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbdbzfdmlx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1h6wxbp</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Pre-Xmas mani 🤶</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6wxbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1h6wlyu</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Sally Hansen insta dri polish and top coat (red bottle) polish not drying even hour later its still denting</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6wlyu/sally_hansen_insta_dri_polish_and_top_coat_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1h6wkyw</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Dragon scales</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xo3u9eh1ix4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1h6wiy5</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>ISO a topper full of green gold scattered holo glitter??</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6wiy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1h6wigk</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Hey Laquerists, where can I buy single mini nail polish bottles?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6wigk/hey_laquerists_where_can_i_buy_single_mini_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1h6vqe5</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Not quite ready to commit to holiday colours yet</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ene8w134bx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1h6vp4q</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Why??</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vp4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1h6v7pi</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first December mani! </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6v7pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1h6v0os</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Treasure ✨🔎✨Hunt</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/un72ls1f5x4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1h6uhsm</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy National Cookie Day! </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6uhsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1h6uha2</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermals + stamping win! </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6uha2</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1h6ug61</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Red to black gradient</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z3dehwy0x4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1h6ufou</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - happy customer :)</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6ufou</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1h6ubj8</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>My 'It's too damn cold out here!' Nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/JzUpJ1U</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1h6ub1m</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gingerbread cookies </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqqzno1uzw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1h6u9mb</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Some Nailpollies love</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6u9mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1h6txxb</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Whats does it look like IRL ?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6txxb/whats_does_it_look_like_irl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1h6tuuq</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Icebreaker Velvetized</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0m7spfb7ww4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1h6tsf2</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>chartreuse speckled polish?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwanqxbsvw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1h6thus</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>A sea of blue-green dreams💙💚</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6thus</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1h6t7d5</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Best brands for non-holo shimmers?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6t7d5/best_brands_for_nonholo_shimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1h6t5cc</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Ilnp compare</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6t5cc/ilnp_compare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1h6slaj</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How am I supposed to give THIS Christmas gift away? </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6slaj/how_am_i_supposed_to_give_this_christmas_gift_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1h6sdkd</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrysknife </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6sdkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1h6sd0p</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tis the season for ice queen nails </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz8vsj69lw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1h6s8vz</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Mooncat Mani</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6s8vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1h6rq83</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Testing new polishes holiday skittle</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gre92w3ngw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1h6rmke</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Aurora Beam 🌈💫</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6rmke</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1h6rh8c</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Nails keep breaking! Help needed</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6rh8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1h6qqjt</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>My first thermal polish, love it, but have realized my hands are always cold</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv3qb25g9w4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1h6qelp</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Mid-way through a mani and I have bubbles in one color, but not the other. Why?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j197qj307w4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1h6q30n</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>We won’t talk about the Thanksgiving nail incident of 2024 that led to the big chop here (or this dry skin offense!)…but we should talk about this multichrome…</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6q30n</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1h6oy8k</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Tree Nails </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/63muo9spvv4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1h6otqh</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Working through my to be read list and untried polishes: BKL's I Invoke Thee</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6otqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1h6omdf</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Growth after 25+ years of nail bitting </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0v4uiz3uv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1h6naps</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Mani </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6naps</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1h6n8l9</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">R.I.P Princess Aurora (dupe wanted) </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oem2ckq9kv4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1h6n7jc</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Galaxy nails</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1xr2opy3kv4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1h6me7n</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>EU Destash Questions</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6me7n/eu_destash_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1h6lps4</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Pretty blue in vague bottle</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6lps4</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1h6lo9f</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Helmers for Sale</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/share/1R1ybut6vQ/?mibextid=79PoIi</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1h6lnqc</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Tanzanite Away-let me deinfluence you</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yagwm9nb9v4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1h6lfu9</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Cool Cat Mom back in stock!</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siqq3gzr7v4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1h6kyej</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>✔️ lived up to the hype</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6kyej</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1h6kw28</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Glistening Gale 🌬️</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6kw28</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1h6krzp</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">big glitter✨ 💖⭐️ </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6krzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1h6kmua</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>how do you guys upload mani pictures without them looking dull in the preview?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6kmua/how_do_you_guys_upload_mani_pictures_without_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1h6jwvr</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Spontaneous Sparkling Grape</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc7v2tcywu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1h6jw99</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When Your Two Mains Collide </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g00nxrvwu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1h6js03</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Anyone have experience with this as a nail oil? It was the only oil I could find with jojoba listed as an ingredient.</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6js03</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1h6jizr</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Mooncat Order</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6jizr/mooncat_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1h6jdqx</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Mooncat Mani! </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzt5hm41tu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1h6ivzg</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Then &amp; now - divorce glow up &amp; tw body talk</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6ivzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1h6iqha</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Storing polish in the basement? Wondering about cool temperatures </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h6iqha/storing_polish_in_the_basement_wondering_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1h6hzj6</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pics of my nails before I broke my ring finger and had to cut them all down to the fingertip 💅🏾⚰️🪦 </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6hzj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1h6hvq2</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>How do y'all store your polishes - especially when you have 40+ of them?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu2b8jt8iu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1h6hn0m</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Thermo polish and Raynauds a tale of many colors ♥️😜</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6hn0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1h6hg90</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Skin that attaches under growing nails (polish photo to protect people who may be squeamish)</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6hg90</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1h6hb9a</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>December means RED NAILS</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6hb9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1h6fwc3</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wject1bb2u4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1h5vebx</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Gelx pressons</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h5vebx/gelx_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1h5vr7y</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">brittle nail help! </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x81iibcqo4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1h66njv</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where did the Essie advent calendar 2024 go? </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c454a6dg4r4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1h6c3js</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Obsessed with these little galaxies on my nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/75t93x20vs4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1h6e309</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Some favs from November</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6e309</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1h6bnf9</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tip for swatch labeling </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6bnf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1h6zmk9</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cirqz6ic8y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1h6ziz1</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Peppermint Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rliiokgf7y4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1h6wsra</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Christmas nails 🧑‍🎄❤️</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ha6gzyujx4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1h6wshh</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I love, spongebob 🪸🦀🪼</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6wshh</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1h6vbf6</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My set of acrylic nails 💅</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6vbf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1h6szdx</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Tis The Season ❄️🎁</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6szdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1h6s0sd</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Winter Nail Set</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6s0sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1h6rxd5</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Nail stand</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1h6rxd5/nail_stand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1h6rjka</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Soft yellow flower nails 🌼</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw5l7ps9fw4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1h6ou83</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>GUCCI NAILS🥀</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5y3t23ohvv4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1h6oqw8</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted snowflake and French tip practice. How did I do?? </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqaergy0vv4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1h6oj7h</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Beautiful</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4j1qk2htv4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1h6oi3z</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">let them glow </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6oi3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1h6nd61</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I think pastels are one of my favorite colors</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6nd61</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1h6lrav</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Smiski nails</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q2xlgsy0av4e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1h6h9uf</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Ya smell like Christmas!!!☃️</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lp44oiidu4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1h6dr3m</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>It's winter, but...</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h6dr3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1h6dmnp</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Absolutely adore florals 😍</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/794jh4apet4e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1h6c3nq</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wish I'd gone all chrome. </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux6tqyi0vs4e1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec  6 08:11:42 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C892"/>
+  <dimension ref="A1:C1084"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15597,6 +15597,3270 @@
         </is>
       </c>
     </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1h7vyrj</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I’m in love with these modelones temp change polishes. Easy, breezy, ombre!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7vyrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1h7vcsv</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>A little help</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7vcsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1h7v9g8</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>First press ons...</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7v9g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1h7v54k</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown nails </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3l2n01r965e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1h7unm4</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>finished my holiday nails! ❄️</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84xykhad465e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1h7tzev</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>how do you gently dissolve nail glue?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7tzev/how_do_you_gently_dissolve_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1h7tfqz</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails and one year free of biting </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo0k4gkkr55e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1h7te35</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>What do ya think lmao</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7te35</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1h7td42</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I have never had my nails done please help</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7td42/i_have_never_had_my_nails_done_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1h7s3w2</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is a replacement for nail polish base? Think sink chemicals replacement </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7s3w2/what_is_a_replacement_for_nail_polish_base_think/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1h7t2wp</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did it😁 </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7t2wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1h7sqr3</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Advice/product advice.</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7sqr3/adviceproduct_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1h7s674</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Starting My Natural Nails Journey</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7s674</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1h7r5by</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw4l685q555e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1h7r2o0</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Alcohol or Acetone for nail prep?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7r2o0/alcohol_or_acetone_for_nail_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1h7qzk9</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>❄️</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7qzk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1h7qipc</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I cannot find a nail salon that can do regular gel polish nicely! What do i get to start doing my nails at home?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tw5995zxz45e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1h7q3u0</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Where do you all get your nail inspo? Need ideas for Christmas nails and AI search results are killing me!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drdwch08w45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1h7pt1w</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a nail twin in here I think👀 either way I love these nails ❤️ just got them done yesterday. </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9gfkotjt45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1h7qdfp</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Nail growth</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7qdfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1h7pz7y</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>$3 press ons!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5hu2rz2v45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1h7pmi7</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Christmas set🎄✨</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7pmi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1h7pgy6</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>First time at nail art</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7pgy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1h7pguq</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails!!! </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7pguq</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1h7n5cv</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>help! OPI gel first time user</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7n5cv/help_opi_gel_first_time_user/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1h7pbhh</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Purple Frenchies</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7pbhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1h7o026</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>What to get done: easiest removal and longest lasting nails??</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7o026/what_to_get_done_easiest_removal_and_longest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1h7n6dc</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I had a gel x nail that totally ripped off my nail. </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biy2eaje745e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1h7ok1h</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Types of nails with no glue?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7ok1h/types_of_nails_with_no_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1h7mmgu</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>How can I fix this?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vto2osgv245e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1h7p6x3</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Best DND gel white glitter nail?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7p6x3</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1h7otwy</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My gel nail designs are always crusty </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7otwy/my_gel_nail_designs_are_always_crusty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1h7onu9</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nail edges lifting </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7onu9/gel_nail_edges_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1h7olru</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htih9093j45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1h7o3jr</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Love my new holiday nails! 🎀</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nadxtvkse45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1h7ne9k</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>The set I did today</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q3sakd66945e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1h7n9gy</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosty set ❄️ </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7n9gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1h7n6l3</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set pink wonderland </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mjxwm4g745e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1h7n4xt</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted Myself SomeJinx Nails (if she wore long stillettos 😝) </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dg33vn2745e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1h7mngw</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red nails with a sparkly snowflake! </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lllrnyn3345e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1h7mj56</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>my holiday nails</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7mj56</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1h7mhzu</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>It's the first time l've done my nails,how did they turn out</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zasm9w7w145e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1h7lkhx</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>My latest! Not a huge fan of them but just needed them done. Shellac.</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7lkhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1h7lieu</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Getting the right mani</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7lieu/getting_the_right_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1h7l3r7</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to be neat and tidy! Festive manicure. </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clwota63r35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1h7kqwd</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Birthday Set!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl2womf9o35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1h7k4jn</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>What nail shape is best for my hands?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7k4jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1h7hh0w</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Can someone PLEASE help!!! (Gel overlay on natural nails)</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey4muzsyz25e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1h7kne8</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas festive nails. </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7kne8</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1h7jch6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Does this shade of blue look good on me?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vznk584xd35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1h7j9nn</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press Ons I Made Last Month </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7j9nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1h7izhh</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New gels #chromebabyblue </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84mi83m7b35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1h7ikt3</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I can’t stop</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7ikt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1h7ih2q</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Nail wraps</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7ih2q/nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1h7iemz</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Winter Wonderland designs from the past couple of weeks❄️🤍✨</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okn84j2x635e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1h7ib04</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails turning colors </t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zv0ki8l6635e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1h7i0sn</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>New set❤️ I’m in loveee</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxfetjy3435e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1h7hy6q</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Clionadh - Psychonaut</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7hy6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1h7hnh7</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>My daily nails 🍃</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mme2iaub135e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1h7hjqd</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Nail ripping from both sides- what can be done?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j9uwsvj035e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1h7hi03</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>🐆 Orange Leo Nails 🐆</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmlpo5v6035e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1h7hdsb</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Did my own</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvibfq37z25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1h7h8ks</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Can I use these as press-ons if there's a bit of a gap?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7h8ks/can_i_use_these_as_pressons_if_theres_a_bit_of_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1h7h7b8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are they supposed to look like this? </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7h7b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1h7gzvn</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Holiday by Bob Mackie - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gzvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1h7gfum</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>So beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjfrs5sds25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1h7gf2g</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Animal print 🐾</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmguixv7s25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1h7gekw</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>🩷🩷🩷😍 sweet</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bpnkez3s25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1h7gaql</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Help! My nails break no matter how short :(</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gaql</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1h7ftea</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>GelX courses</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7ftea/gelx_courses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1h7fs2o</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Simple Christmas Set</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1rw6w3in25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1h7fetr</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>New Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7fetr</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1h7f8bk</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gingerbread cookies </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22vw1drjj25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1h7dngk</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Application</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ddmou1dv725e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1h7d9cx</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Overfilled near the cuticle</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7d9cx</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1h7d9ci</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>I know its December, but I could not resist an animal print moment ✨</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2w80dzy425e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1h7bcec</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>My salon Gel-X nail fell off after only 5 days :(</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7bcec/my_salon_gelx_nail_fell_off_after_only_5_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1h77m1b</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Injury to nail bed 6 weeks ago</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kqsnbeks05e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1h74v5v</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>made these nails for a coworker, i have never really tried or been good at designs. but here’s mine compared to “professional” nails i got done for $85 a few months ago… i still regret that purchase because girl..</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h74v5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1h7cvz8</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>One month later!!!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7cvz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1h7btzn</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fall nails that will be on til the 20th 😆 </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7eqd6u5u15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1h7axe2</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Good LED lamp to dry nail polish ?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7axe2/good_led_lamp_to_dry_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1h7at39</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Glow in the Dark Winter Glam</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h7at39/glow_in_the_dark_winter_glam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1h79vay</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Red cat eye.</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz6mjtj5e15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1h79q2a</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Christmas nails!! Simple ✨</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h79q2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1h79lx2</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They are beautiful </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehyq6xgyb15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1h79l0z</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Snowy🤍</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/32cn9cgqb15e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1h79e74</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h79e74</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1h79bro</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic Rose french </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3phrg2e915e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1h77jau</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Gold Nails✨</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k38gltsr05e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1h777tr</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Pink candy cane nails</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h777tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1h76ucc</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Ireland - LF Semi Cured Gel Nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h76ucc/ireland_lf_semi_cured_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1h75jso</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Christmas nails in red ❤️</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epaoef1e305e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1h75bwf</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>REGULAR polish cherry glazed nails 🤩</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4f20h5g005e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1h74nsj</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Please help me decide! ♡</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h74nsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1h74ob8</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>New Set For Christmas😌</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h74ob8</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1h7uozn</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Does Tonic Polish no longer exist?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7uozn/does_tonic_polish_no_longer_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1h7uesx</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ordered bundle from ILNP on Monday and it's still processing. Is this normal? </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7uesx/ordered_bundle_from_ilnp_on_monday_and_its_still/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1h7txnc</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fake nails for 11 yr old. </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7txnc/fake_nails_for_11_yr_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1h7tfqh</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Black Cherry</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/black-cherry-dec-2024-md403vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1h7t1y5</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>November nails! 🍁🦃</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7t1y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1h7t0lu</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Elegant gold magnetic</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7t0lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1h7s5eq</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Visionary- LLP</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7s5eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1h7rsaq</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Mooncat cracked bottle?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th3ajstlb55e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1h7r8on</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Big Sagittarius Energy </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7r8on</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1h7qtp4</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2025 Pantone Color of the Year: Mocha Mousse </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7qtp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1h7qlet</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>How to tell what undertone a nude is</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7qlet/how_to_tell_what_undertone_a_nude_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1h7q6cx</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>This one just gets me 😍</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl2of4nuw45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1h7q5e8</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Mooncat “Root Of All Evil” is stunning!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7q5e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1h7pudi</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Magnetic Polish hack! Pipe clamps!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7pudi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1h7piex</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My sassy sauce haul is here!!</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yghvm0dvq45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1h7on71</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>I got glitter in my top coat. Is it ruined?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7on71/i_got_glitter_in_my_top_coat_is_it_ruined/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1h7oeew</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>First holiday set this season!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7oeew/first_holiday_set_this_season/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1h7o8tz</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">G'day from Australia! </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7o8tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1h7narx</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>BF package made me scream</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7narx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1h7n1kz</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to ILNP </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7n1kz/new_to_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1h7mv3w</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Handbook for the Recently Deceased - Clionadh Cosmetics</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bf70lbfq445e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1h7mpk7</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>first indie/boutique purchase: holo taco secret society!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7mpk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1h7m81e</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>ILNP Kiss &amp; Tell hits right in any light 🤩💕</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7jkez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1h7l0x0</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Excited to have finished another bottle! Want to know how many uses it took?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7l0x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1h7kovs</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish+top coat peeling off in one chunk after 5 days but base coat stays - how do I fix this? </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7kovs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1h7kktn</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">accidentally ruined nails </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b3v1em0n35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1h7kioh</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>In loooveee with DND French Raspberry 066</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7kioh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1h7kh64</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>sleepy hollow by polished for days 🎃</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9asklo89m35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1h7kfy2</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Trying to summon a snow day with a snowy manicure.</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7kfy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1h7jf8z</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First of the season </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1arxgiphe35e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1h7if65</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Cool Cat Mom vs. Chesire Cat</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7if65/cool_cat_mom_vs_chesire_cat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1h7icio</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve">swipe to see my nubs from a few years ago 😳 </t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7icio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1h7hym0</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Clionadh - Psychonaut</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7hym0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1h7hh78</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Exfoliation took the shine off my topcoat. </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7hh78/exfoliation_took_the_shine_off_my_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1h7h7lm</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>First Dec Mani</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7h7lm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1h7gzsj</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I’m a sucker for iridescent white polishes 💖</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gzsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1h7gu7b</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Thermal question</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7gu7b/thermal_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1h7grsw</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>My BF order arrived, so I'm gonna share my feelings with you 🤗</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7grsw/my_bf_order_arrived_so_im_gonna_share_my_feelings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1h7gcim</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My Thanksgiving Nails (did them late that night and haven't done anything new yet)</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gcim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1h7gb47</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Bouquet toss</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gb47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1h7gaaj</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gaaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1h7g6bk</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Got The Blues For Red</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7g6bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1h7fyle</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Has anyone else not gotten a confirmation email from INLP for their black friday order??</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7fyle/has_anyone_else_not_gotten_a_confirmation_email/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1h7fvhj</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV light sensitivity? </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7fvhj/uv_light_sensitivity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1h7flkb</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Trying to match Pantone’s Color of the Year 2025</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7flkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1h7fkoq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Gel Gold Shimmery Topper?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5yamkozl25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1h7fcas</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expressie misfit right in </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7fcas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1h7fbzg</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's finally here 🙌 😍 </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7fbzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1h7fabo</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Browns like Pantone 2025 Mocha Mousse?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7fabo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1h7f8sc</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>…and so the cycle continues😭</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f43tuconj25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1h7epqy</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Dupe for GLL - I know that pain and I won’t run away like I used to”</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7epqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1h7emvm</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>I’m looking for the perfect nude for a French mani</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2rhu7b6f25e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1h7egn9</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Taking advantage of the cold with thermals! 💕</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7egn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1h7ea18</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Only 1.98 for a color this pretty?! Thank you L.A. Colors 🧚🏼‍♀️🤍</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7ea18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1h7e5is</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Lust for Vengeance</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7e5is</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1h7e4fk</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Almost festive by accident</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89bmdbefb25e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1h7dple</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my office lighting! </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7dple</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1h7d3ij</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My Polished For Days BF Haul</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7d3ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1h7cko2</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Looking for this glazed/shimmery colour. Any ideas what this would be?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqhqj10vz15e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1h7cjqi</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Yes, you DO need KBShimmer's "Tricked Out"</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ey13yqiz15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1h7cigc</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>From my cuticles to yours…. Thank you🙏🏻</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40gtgteez15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1h7buux</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Essential gift ideas for wife</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7buux/essential_gift_ideas_for_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1h7bq7u</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Mooncat + Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7bq7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1h7be6a</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Starbucks Green ☕️</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7be6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1h7as16</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Getting into the spirit with some holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7as16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1h7aozb</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Seeing them all at once makes my heart happy. So glad I swatched!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zas63ry4l15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1h7aalb</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>The sun changed my cuticle oil from yellow to clear/colorless. Is that bad?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0txq9esh15e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1h79tsu</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Betelgeuse over Jet Setter and my cat, Spook</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h79tsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1h79kkh</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Office Christmas party today</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h79kkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1h78wv5</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Finally, a white polish I love ☁️Memento Mori 🤍</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h78wv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1h78cmh</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>RIP Nail</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvvaxf07015e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1h780go</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h780go</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1h77eeq</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Gel polish always peels off</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h77eeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1h75ysa</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first attempt at velvet- how is it? </t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u44y2oiv805e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1h75xe7</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Impatiently waiting for my black Friday purchases to arrive!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4vaw6ae805e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1h75su5</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Colour me impressed 🤩</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mcj9kzjs605e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1h75qzo</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>💜 Purple 💅</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ppe7ll3605e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1h7tm2f</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>What is this style called??</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7tm2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1h7p24x</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>What do you think? Do you like hearts?🩷</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nigpf4hvm45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1h7oqpo</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7oqpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1h7o5r5</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Help from the girlies is needed ASAP!!!!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mlfhwdbf45e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1h7n4og</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted Myself SomeJinx Nails (if she wore long stillettos 😝) </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16t65ej0745e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1h7j1tm</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas nails! (And the Thanksgiving nails I had before) </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7j1tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1h7imfj</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Animal Crossing nails 🐾🌸</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7imfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1h7igpo</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Christmas light nails pt 2</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ws60w78c735e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1h7i6l3</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>something from today ☀️</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ldaxfsa535e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1h7hrme</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7hrme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1h7hhmk</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>🐆 Orange Leo Nails 🐆</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pntjy274035e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1h7gy7s</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Holiday by Bob Mackie - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7gy7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1h7fs1h</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Feeling festive 🎄</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7fs1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1h7f0ax</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>silver perfect for a cocktail afternoon</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7f0ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1h7bjaa</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmlcga2vr15e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1h7a0ol</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>chocolate rose gold chrome nails! done by me :) swipe for my inspo 👉</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7a0ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1h78zko</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Christmas light nails!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hpr467y9615e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1h782oi</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>second set of nails!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpkhbv7fx05e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1h75krt</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l87a847r305e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec  7 08:10:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1084"/>
+  <dimension ref="A1:C1268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18861,6 +18861,3134 @@
         </is>
       </c>
     </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1h8npsh</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">strawberry nails 🍓 </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8npsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1h8m94o</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om03ts9ybd5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1h8lzvu</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>My fingernail is growing wrong and idk what to do. Does anyone have any advice on this?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2p2n5909d5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1h8lwnl</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No airbrush needed </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpghrk8y7d5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1h8l3jk</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>My Christmas set</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8l3jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1h8kpzv</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>New nailsss</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8kpzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1h8kjg7</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Xmas Nails w/DIY Snowman </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx9vvx7xsc5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1h8jrjh</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wedding nails! </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uah8bm00lc5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1h8jnv0</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Didn't get the good nail gene so I finally thought 'screw it', painted my own plastic nails, and glued 'em on</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8jnv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1h8itny</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Easy Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8itny/easy_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1h8hb2j</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would a nail salon like this go huge or go under? </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8hb2j/would_a_nail_salon_like_this_go_huge_or_go_under/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1h8gxgg</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>My sets this fall 🤎</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8gxgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1h8grl8</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Classy Christmas set❄️</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8grl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1h8gqb4</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>New Set!❄️</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xyvyfcr4sb5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1h8gora</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>DIY “Snowy Mistletoe” nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ugpivohrrb5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1h8gb10</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternatives to acrylics? </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8gb10/alternatives_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1h8func</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Best Gel nail kits?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8func/best_gel_nail_kits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1h8feoi</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>I get my nails done with clear gel about once or twice a month</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8feoi/i_get_my_nails_done_with_clear_gel_about_once_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1h8fmh5</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tycq0nfcib5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1h8flp6</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ooyxjny4ib5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1h8fdw2</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using gel polish. </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8fdw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1h8fdht</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is a 30mW/Cm^2 UV Lamp ?? And Can i use it, does that convert to Watts  ? </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8fdht/what_is_a_30mwcm2_uv_lamp_and_can_i_use_it_does/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1h8f8qe</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Can I ask my nail tech to remove nails she just did?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8f8qe/can_i_ask_my_nail_tech_to_remove_nails_she_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1h8f88h</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Can I use Holo Taco Peely Base with gel nails?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8f88h/can_i_use_holo_taco_peely_base_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1h8f6mm</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>My kiddo picked my Christmas nails! I loved how they turned out!</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnji3t5keb5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1h8f2ue</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Help! I want all of my nails the same but can’t decide which style for Christmas. </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8f2ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1h8f15h</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Christmas nails 💅 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikx6k1r6db5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1h8eytn</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>simple christmas nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8eytn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1h8dum2</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Peeling gel</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8dum2/peeling_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1h8eirj</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8eirj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1h8e2wc</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>December Nail Art</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tai1c1375b5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1h8e0g2</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>We love some Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y450i7hm4b5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1h8dysw</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun lips and a heart </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8dysw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1h8dl4s</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>trying something else than almond with french tip, does it looks good?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8dl4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1h8cvd4</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>PRESS ONS vs GEL</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2bp4s7eva5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1h8d767</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>More colours is always a good idea for a gloomy day 🍂</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dq9bchmxxa5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1h8cxk0</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Holiday set</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gxxmwnvva5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1h8csf3</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Interesting foil Christmas nails. The green glitters in different light. </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8csf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1h8cqn5</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is nail glue safe to use on bitten nails? </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8cqn5/is_nail_glue_safe_to_use_on_bitten_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1h8cphe</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Christmas sparkles…but make it 🖤🗡️🕯️</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6rcbln3ua5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1h8cnbg</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>I botched the candy canes but I still like how it turned out :)</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8cnbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1h8bw6p</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>🩷🩵 Rogue Laquer It Glows ✨</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8bw6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1h8b96a</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Removed glue on press on nails for the first time and nails look like this now. How can I clean off the "residue"?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh9kg9ykia5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1h8b58a</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>They are a week old but I’m still obsessed with my gel-x brown chrome mani 😍</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qgf2djpha5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1h8a4n6</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>This post is called “I’ve finally decided to find a private nail tech.”</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmha80dq9a5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1h8awkx</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried a new nail salon and had a bad experience </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8awkx/i_tried_a_new_nail_salon_and_had_a_bad_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1h8av4d</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Xmas nails </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8av4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1h8aqt9</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>my nails back in July 🎀</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jymt1llhea5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1h8aoy6</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Drippy nails!!! (Ty for all the xmas lights nail love, guys!! My ADHD made me do adrastically different style on my other hand 😊)</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8aoy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1h8al7i</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got dipped </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8al7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1h8aawy</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SOS leaving for vacation in 12 hours </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otipo2n1ba5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1h8a18a</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails alternative </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtzv6uyz8a5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1h89zrg</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Not bad for press ons</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w1bs8vo8a5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1h89oz9</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons and super glue </t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js9ukvwd6a5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1h897mb</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails 💅 </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn9y1opm2a5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1h8927s</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>this shade of red 😍</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfx4kyhi1a5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1h88rex</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling a bit festive </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rx7uqqaz95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1h88457</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting acrylics </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c82hiivcu95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1h87z2d</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Christmas is the perfect excuse for a new set</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2c0lcx9t95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1h87ww5</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>So proud of my grown out nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87ww5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1h87shv</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Can you cut and shape press ons?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h87shv/can_you_cut_and_shape_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1h87ni0</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did I do? </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87ni0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1h87hnv</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>My Christmas nails!! 🎀❄️</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlrjq9ynp95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1h87gs8</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Simply white and gold</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq89bhkhp95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1h87fpg</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Blush pink nails are so cute 🩰✨</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87fpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1h87bqz</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My cat stole the spotlight here </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eor544iho95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1h879tq</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Do you like the color it gives with the effect?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a15labl3o95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1h86zmc</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Dupes for essence’s colour &amp; go in the shade space queen?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h86zmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1h86xv9</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Is it too late to post my fall set 👀</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28qofeiml95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1h86pbm</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Festivus nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h86pbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1h85qlj</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Didn’t really want Christmas nails 🔮✨💜</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h85qlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1h85ixt</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Christmas nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h85ixt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1h85i7j</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>What to ask for</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h85i7j/what_to_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1h8568s</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Icy blue with sparkles</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8568s/icy_blue_with_sparkles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1h84irt</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok, I'm trying </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h84irt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1h84h48</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Christmas Cookie Set of press ons 🎄🍪 (plus the inspiration)</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h84h48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1h81jl2</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Vertical nail crack</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xux6y5uoe85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1h83l8e</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried water marble effect for the first time. </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h83l8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1h82o7k</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye nails </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8iaoaa8ko85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1h82l9q</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>I am a man who wears nail polish. I also have a YouTube channel where I build computers. These are some of the comments on my latest video 😂</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h82l9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1h82ckx</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>☠️ Sugar Skull Nails ☠️</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/903j0n0rl85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1h810lu</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h810lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1h7zbk4</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>floral blue cat eye nails for my thailand trip 🌸💙</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edkyzcxrr75e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1h7yz0b</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>just shaped and painted my natural nails! can't wait for them to reach my longest length 🥹</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7yz0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1h7x2oj</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Delicate flower nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7x2oj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1h7wvn1</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you for everyone's opinion🥰! I did the glow in the dark christmas light nails! </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7wvn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1h7woqo</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>I cannot for the life of me do a peppermint</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7wv33j7t65e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1h8nw3p</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>baby's first square mani</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8nw3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1h8noi1</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HT Moon Lagoon dupe? </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8noi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1h8me8z</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>After a big break, we're starting fresh with shorties</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93ubpc9mdd5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1h8md1v</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatch Comparison Request - Holo Taco Head Hunter and Devils Advocate </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8md1v/swatch_comparison_request_holo_taco_head_hunter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1h8m59l</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Starry night nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8m59l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1h8m0p7</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Polish pickup?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8m0p7/polish_pickup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1h8lfbj</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Subtle silver snowflake-y nails (pre cleanup)</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8lfbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1h8l4mq</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Polish to match my cat's eyes?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3a7a529zc5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1h8jwsu</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Told the Northern Lights to Keep Shining</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6odlolhmc5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1h8j4ft</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Ghosts of Hecate</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8j4ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1h8i3z2</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love having girly nails while going not-traditionally-girly stuff. Anyone else? </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8i3z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1h8hr7j</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>what to do with unwanted top coat?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8hr7j/what_to_do_with_unwanted_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1h8gxji</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Mooncat Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyjhdwvxtb5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1h8gwh6</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Trying to choose an ombre to do</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8gwh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1h8gmtu</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>How to help grow my nails</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8gmtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1h8gl6k</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I am sooooo late to the Rosewater Jelly party, yay for black Friday sales!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8gl6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1h8fxlu</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>I want a color that reminds you of tattoo ink?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miji2nm3lb5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1h8fl6z</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>moonbow 🤩</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8fl6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1h8fbg8</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Trying to squeeze a christmas mani out of my very spring/summer polish collection</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8fbg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1h8f8au</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Regular polish</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7v4e6myeb5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1h8er4k</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Please enjoy this second installment of topper experiments</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8er4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1h8enys</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Red for the holidays? How groundbreaking!</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mtoao40ab5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1h8eglk</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>ILNP — Pixie Party</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8eglk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1h8eaw9</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Can someone explain how I just got my two largest BF hauls ever and instead of feeling sated I instantly want more? 😬</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8eaw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1h8dm4l</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>✨️❄️Snowy Sparkles❄️✨️</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8dm4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1h8dka1</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer shipping update </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdu5mvzv0b5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1h8cs3v</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>First shot at Christmas nails!!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8cs3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1h8cqrq</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Looking for a polish dupe</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8cqrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1h8c8nu</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Help, I've Fallen 💜🧡</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8c8nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1h8c87g</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first I Scream Nails BF order. I had no idea they had such cute packaging! </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8c87g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1h8c6bg</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Cirque - Elixir of Everlasting Life</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjypwqhvpa5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1h8btw9</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>🩷🩵 Rogue Laquer It Glows ✨</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8btw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1h8b5fq</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>I mixed all of my polishes together</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8b5fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1h8auc7</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>My turn for the Wicked mani!</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4coqdc8afa5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1h8asyi</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>OPI Glazed and Confused. Excuse my already winter cuticles</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jmcp4zyea5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1h8aibt</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Does anyone know what shade this Emily de Molly polish is? (Violet in the middle)</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbfykf9nca5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1h8ahh5</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Please help! 2 of my real nails are cracked deep in the nail bed all the way across after getting my first ever gel manicure. (First manicure in 10 yrs) I dont know what to ask the nail salon to do. Please help!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8ahh5/please_help_2_of_my_real_nails_are_cracked_deep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1h8ahbk</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Sacrificial Lacquer 🥀 (I'm obsessed)</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8ahbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1h8acga</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Decided to try out the circle part of the magnet</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8acga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1h89g8g</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Favourite drug store jellies?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h89g8g/favourite_drug_store_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1h88h41</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Christmas skittle inspired by one of ILNP’s posts. </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h88h41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1h88gqg</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>ILNP haul</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na4nv2gzw95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1h87yxa</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>ISO: magnetic holders that let you hold bar magnets at fixed angles</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h87yxa/iso_magnetic_holders_that_let_you_hold_bar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1h87d7m</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MC, HT, Cirque swatch comparisons </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87d7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1h87c3s</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Pictures don't do justice ✨️</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87c3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1h87b8g</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Such a cute idea from Cracked!!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3hfc7ndo95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1h86ey3</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Holo Taco leak (official 😅)</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uzo778kh95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1h868kl</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dup for holo taco cloud nine? </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/649fr0w7g95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1h866jw</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vaguely festive :’) </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2icn3eosf95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1h85o9e</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>How do I better care for my nails and skin around my fingers? Working on getting my nails longer for polish</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h85o9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1h85nbs</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>how often do you paint your nails?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h85nbs/how_often_do_you_paint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1h85g7o</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Holiday spirit nails: Sinful Colors “Sugar Sugar”</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h85g7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1h856ka</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wore 14 colors in November! </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h856ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1h84o15</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Just got my BF Holo Taco haul!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu6hzhkc495e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1h84jh1</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Another TJ Maxx/Marshalls hidden gem?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbwozycd395e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1h83vmf</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let the festive manicures commence! </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1il43zx8y85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1h83uci</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Monster Peach/Flicker Conspiracy</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h83uci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1h836sg</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Dazzle dry and mooncat nail polish my</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7bnmt1ts85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1h835sz</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Easiest velvet nails so far</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f7b1u7ahs85e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1h8355w</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>non-shrinking qdtc?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8355w/nonshrinking_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1h82zry</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else just admire their own nails when it turns out good?? </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq7j6w28r85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1h82wvn</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Rainbow Connection (UK) postage</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h82wvn/rainbow_connection_uk_postage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1h7femt</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Nail Polish Weakness</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h7femt/nail_polish_weakness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1h82s12</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>HT topaz tears worth it?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lugxt4hp85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1h82czw</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Madam glam dupe</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfdywvlul85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1h823bh</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Idk how I feel about this one! </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/llui42zcj85e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1h81f2p</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Stretching my Sunday mani</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h81f2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1h811zx</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Birthday nails✨️</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h811zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1h80b0q</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zhtp6lq285e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1h7zm9p</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Fox Nails </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7zm9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1h7yolg</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Mooncat isn't Amazon Prime</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>/r/mooncatpolish/comments/1h7whlo/mooncat_isnt_amazon_prime/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1h7xkla</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Serpents of Eden is AMAZING</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adfnn5k6575e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1h7x72f</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>I am so in love with my nails</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7x72f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1h7wpws</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Mooncat-After the Rain🩵</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h7wpws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1h8nw10</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Loving my new DND Gels!</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/44zjclwfwd5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1h8lens</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Is there any way to clean sweater nail designs?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4x54r8y72d5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1h8iohq</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>They took me almost 3 hours 😅</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41rthtlaac5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1h8fcwj</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Gingerbread nails</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aeawbnj1gb5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1h8cil7</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I made my mom for Christmas </t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8vcvz8lsa5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1h8c4kr</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anime Danganropa!! </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnuly71ipa5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1h8bdxm</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails! </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3qtivtmja5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1h8awxx</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">green perfect for this season </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8awxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1h8at7w</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Xmas nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8at7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1h89kas</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two different vibes both totally Christmas!! </t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h89kas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1h894s9</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h894s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1h87j1j</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Winter wonderland 2024</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h87j1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1h8722t</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Que les peace, yo am 😍</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8rh1p1im95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1h86dpd</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a different combination </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvtkb172h95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1h8621m</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>add a lot of colors to your life</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8621m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1h84g72</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>December nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bai6i7p295e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1h83lci</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Matte black "smokey" nails</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h83lci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1h83la4</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Winter Wonderland</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krrwks0zv85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1h82cd6</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>☠️ Sugar Skull Nails ☠️</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3ynse8pl85e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1h817ql</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Definitely the most complicated design I've done to date</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h817ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1h7xsi8</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>First Christmas set of the season!!!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqh8otf8875e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1h7cqy9</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Island vibes</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sp0c6l2125e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1h6rhf6</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I love them.. I try</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1rhu04uew4e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec  8 08:10:18 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_08.xlsx
+++ b/data/collected_data/2024_12_08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1268"/>
+  <dimension ref="A1:C1468"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21989,6 +21989,3406 @@
         </is>
       </c>
     </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1h9dsj3</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>I like my new French manicure</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/farp0fxlwk5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1h9dgmg</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>pink n spooky</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9dgmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1h9del9</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Fresh nails</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjwrv89rrk5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1h9ddrg</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>christmas nails dropped</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8tdtk4grk5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1h9cvp5</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>My nails are soft and break easily :( any advice?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9cvp5/my_nails_are_soft_and_break_easily_any_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1h9cnek</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Simple Christmas French tip :)</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djy1aqqeik5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1h9bmp3</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>How do i change the drill bits?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm7cnc0r6k5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1h9c5us</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So festive! </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9c5us</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1h9bwth</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>tried to do mildly ghostbusters themed nails with my bad skills and even worse supplies</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9bwth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1h9bfm6</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My absolute favorite set I’ve done for myself so far. </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuass83l4k5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1h9b772</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Nails over filed?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9b772</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1h9az4b</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic or gel? Which is better? </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9az4b/acrylic_or_gel_which_is_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1h9a4lf</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>How to make press-on nails last longer?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9a4lf/how_to_make_presson_nails_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1h9a2bf</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>It's beginning to look a lot like Christmas ☺️❄️</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9a2bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1h99rww</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>My progress</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h99rww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1h99evc</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Recs for a brand of press ons that won’t destroy?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h99evc/recs_for_a_brand_of_press_ons_that_wont_destroy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1h99ao8</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>First time frenchies 💕 not perfect but very bright and fun</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsgi2k2thj5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1h98mpe</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Beds Question </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h98mpe/nail_beds_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1h98tzo</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr6zny0ydj5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1h98h6o</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Strongest/most durable BIAB?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h98h6o/strongestmost_durable_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1h984u4</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me with my wedding nails! Inspo pics from Belaya Nails on Pinterest </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5t8ktj57j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1h98emr</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Month nails 🎂 </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h98emr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1h986el</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Red polish and a matte top coat on my natural nails, I'm so happy!!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h986el</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1h982kp</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Holiday Sparkle</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rspmhghf6j5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1h9822s</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>If I want to see the polish colour on top of the lid</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h9822s/if_i_want_to_see_the_polish_colour_on_top_of_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1h980kz</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>New Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h980kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1h97xrz</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>I’m so sad…</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h97xrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1h97umm</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails are ruined from gel manicure help </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df7okl2d4j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1h97kpx</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black &amp; gold for the festive season -- DIY hard gel </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/od4cujtr1j5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1h97ge7</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Rose gold nails</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkke49po0j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1h97fuz</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude Ombré </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h97fuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1h97f3z</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new mantis loves my scorpion set! </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyf0z6xc0j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1h95bjv</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>New manicure, need tips for gradient/ombre</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95bjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1h95mj2</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>hard gel vs acrylic at home (peel off base)</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h95mj2/hard_gel_vs_acrylic_at_home_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1h96570</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Please Help Me Know Where I Went Wrong</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h96570</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1h976py</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h976py</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1h96xyq</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Wide nails help</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3cbujkzvi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1h96rdf</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Xmas and New year </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h96rdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1h96hmx</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Second set of press ons</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h96hmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1h96cvx</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Any ideas?</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h96cvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1h96bva</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I didn’t hold back </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psx3f0qiqi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1h966gd</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Love My Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h966gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1h95sqn</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Glam Christmas by me ✨🎄</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95sqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1h95cs0</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>My nail tech didn't fail me</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/umju6fewhi5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1h95c76</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just love it. </t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tknpmydrhi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1h95c3f</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Because an apocalypse won't stop me</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5k1lqfqhi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1h95b3l</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Gemmed Out! 💎 💜</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95b3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1h94ku7</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>My manicurist made me gleam ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cbd9cq5bi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1h94ezm</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>I'm very much in love with this design but this month they're going🥹</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h94ezm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1h94dm7</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>tis the szn</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc8poy0e9i5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1h94ayi</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Does anyone have an idea of what this is!?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvd8rp5r8i5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1h933pv</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Growth progress after nail got ripped off</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h933pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1h93jgs</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Christmas!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h93jgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1h93g4v</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my maximalist dream </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h93g4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1h93bjx</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>pink on pink 🌸🧚‍♀️🌺💖 very glinda coded</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhobn7af0i5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1h938il</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>All blue for holidays</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u9dfz1qzh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1h935lx</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Is my manicure putting you in the New Year's mood</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbcx0fnwyh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1h930cr</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Opinion on these?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h930cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1h92z7i</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>apres milky way galaxy 💙🌌</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h92z7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1h915ul</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>What am I doing wrong? - builder gel</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h915ul/what_am_i_doing_wrong_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1h92o2l</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Quick press on set with Curv Life semi solid glue</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la76kdqxuh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1h921hi</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcly6oqlph5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1h91ybn</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Love it!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h91ybn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1h90wle</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>First two Christmas sets! (I can’t do more than two weeks between fills…)</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h90wle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1h90tc5</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Obsessed with Deep Space</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nqbfgymfh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1h909qs</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>What glitter do you think goes best with this nail color?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dunddej6bh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1h909l8</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Jinx from 'Arcane' Nails</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31c8ds75bh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1h906x5</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>‘Tis the Season🎄🎅🏼🎁</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h906x5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1h904up</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Xander as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h904up</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1h90022</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Chrome for the holidays</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h90022</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1h8zzlj</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Regret and Love</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8zzlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1h8zvs2</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Capricorn season coming in soon! (OPI Capricorny)</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2jivq608h5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1h8zlrh</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Got my nails done and one fell off less than two hours after</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8zlrh/got_my_nails_done_and_one_fell_off_less_than_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1h8yl2n</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>My Christmas Set</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yl2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1h8zmqd</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Some swimmers for summer</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8zmqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1h8y5gm</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Can i do acrylics at home with picked at cuticles?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8y5gm/can_i_do_acrylics_at_home_with_picked_at_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1h8zj9f</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>North Pole Chic</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7hq8rf95h5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1h8zd4m</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help?! Smashed thumb advice. </t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8zd4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1h8yxls</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>In mood for Christmas nail art 😃</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj4lty0g0h5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1h8ytox</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>First time getting extensions!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8ytox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1h8yqq8</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>First time getting extensions!</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yqq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1h8yo0j</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze83yofdyg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1h8yng6</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>off to the city :3</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yng6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1h8yl18</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>I haven’t had my nails this short in years, but I kinda like them ❤️</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w849g71qxg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1h8ykiu</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>My Christmas Set</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8ykiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1h8ykf6</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’m in love with these colors </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/794ibhllxg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1h8yjyt</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>My new favorite set 💕</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yjyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1h8yjtu</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>My new favorite set 💕</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yjtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1h8ygip</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Tis the season ♡♡</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8ygip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1h8y7wf</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Christmas French? It took almost 3 hours but I love it 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0cjaaztug5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1h8xxf3</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>holo taco declassified 002 swatches (contains gifted pr)</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8xxf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1h8xvyi</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>I’m in love with these press-ons I painted!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i3cely8sg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1h8xqjc</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set </t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqb2abtzqg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1h8xh3b</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Taking a break from gel polish — looking for product recommendations!</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlmfodwtog5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1h8w9pn</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Ocean inspired Nail art 🌊 Loving this fresh and breezy design</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8w9pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1h8ufv5</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Nails lifting not even a day after getting them..</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wgs7usuzf5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1h8rhq7</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Fill w/ length?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8rhq7/fill_w_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1h8xh67</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Ridges In Nails?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1h8xh67/ridges_in_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1h8xgvs</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My December nails </t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5byr4oxrog5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1h8xg2k</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>What is wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8xg2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1h9dl25</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Period polish</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9dl25/period_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1h9dcyu</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Natural nails delaminating.</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9dcyu/natural_nails_delaminating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1h9czxi</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>the easy velvet hack works so well!</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/69hea4qpmk5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1h9c07z</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some holiday flair </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsnsz6cxak5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1h9bots</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>I can't even capture how amazing...</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9bots</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1h9ay1a</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>i'm trying to give my husband christmas ideas and i'm stressed help!!!</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9ay1a/im_trying_to_give_my_husband_christmas_ideas_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1h9afbt</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To whoever posted about Notion this morning... </t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qxm7pm4uj5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1h9a8d0</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Anyone know this lilac shade or something similar?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcey1427sj5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1h9a87e</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Request: ILNP Encore over ILNP Shapeshifter?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9a87e/request_ilnp_encore_over_ilnp_shapeshifter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1h9a2du</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Swatchers to follow?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h9a2du/swatchers_to_follow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1h99swf</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Couldn't find any nail art i liked for Christmas so I accidentally discovered this nail combo instead [products listed]</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hi6jbt6pnj5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1h99hoq</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>🤤Mmm mmm mmmmm😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbfh1kthkj5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1h99fuw</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>First Christmas mani</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h99fuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1h9917u</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>My Wicked Mani 🧙‍♀️</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9917u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1h98wwz</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Alright y'all, I need your help finding a polish. Brian David Gilbert is wearing an AMAZING copper/green multichrome and I have to have it.</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h98wwz/alright_yall_i_need_your_help_finding_a_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1h98vbq</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reflectives? </t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sge9hy8aej5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1h98mwa</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>creds to mooncat for making me fall in love with a creme</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h98mwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1h98kiq</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Mooncat’s Emo for Life and Millennia 🖤🌌🛸</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h98kiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1h98hws</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Phoenix - Teleport</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h98hws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1h98ah7</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>am i crazy for thinking that shimmers almost always look better in just one coat?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h98ah7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1h98710</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Perfect raspberry??</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h98710/perfect_raspberry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1h980gx</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>I’m so sad…</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h97xrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1h97zdv</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Help with drying - mooncat</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h97zdv/help_with_drying_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1h97mhi</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails from revlon </t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvej77982j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1h97hpf</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>winter vibes❄️</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h97hpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1h97esf</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone seen one of these organizers in any color? I've looked at a lot of them and I've only seen them made in clear acrylic </t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/236pa8t90j5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1h974sa</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 question</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h974sa/nailtiques_formula_2_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1h96s3x</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bkl - Heir , looking like a field of stars </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h96s3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1h966mx</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please Tell Me Where I Went Wrong </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h966mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1h965yg</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>WE KEEP GETTING MORE</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvmvq113pi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1h9629e</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My first ever order from ILNP. 20 swatches from my Black Friday Haul.</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9629e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1h95xe8</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Glam Christmas by Me ✨🎄</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95xe8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1h95ki2</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>I was influenced by this sub</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95ki2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1h957gx</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Anyone else not feeling Christmas-y?</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h957gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1h94mui</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Red glitter on black</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f57uz2mbi5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1h94ctx</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Matching my Christmas decor</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h94ctx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1h94bm9</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Loving the color shift on this one</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rwo1yjkw8i5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1h9448z</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I reorganized my display shelves </t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9448z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1h93l3a</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Sassy Sauces- Mystery Bundle! </t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ufc7sm2i5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1h92sse</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>am I everything you fear ft. shorties</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq9wgcc1wh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1h92mfv</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>It’s very hard to pose two bottles</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h92mfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1h92fx0</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple Metallic </t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h92fx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1h9240p</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still in love with the ILNP overcast collection </t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heqn4td7qh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1h90vex</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Slots of Fun - Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h90vex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1h909xv</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Snowflake vacation mani</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq8i4528bh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1h907sj</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>is this color out of season?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h907sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1h900jb</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Regret and Love</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h900jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1h8zuag</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a big change! Went from tapered square to pointy! </t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8zuag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1h8zoql</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>OPI It's The Shiz. Am I the only one excited for this one? Mine comes Monday I think with 2 other Wicked collection colors).</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q88h5ig6h5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1h8zakj</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Heat resistant nail polish?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8zakj/heat_resistant_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1h8z7jq</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">christmas is here! nails for caroling 🥰🎄 </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8z7jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1h8yse5</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>House of Hades, I know, how original</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8yse5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1h8ychv</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>am i everything you fear?</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6ao88cuvg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1h8y48h</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Sygar Rush with Everything Taco 🤍 🌮</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbndfbp3ug5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1h8y1ic</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>holo taco declassified 002 swatches (contains gifted pr)</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8y1ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1h8x8ix</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Black Friday Haul</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psuuxmdxmg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1h8wn1a</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Festive nails!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8wn1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1h8vicx</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>{PR}✨ Introducing Midnight Rendezvous ✨by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8vicx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1h8vhwh</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Obsessed with this holo!</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8vhwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1h8vdfv</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Finding the right shade of red</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8vdfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1h8v4qr</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Velvet Molten Sky</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8v4qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1h8v2mz</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Back to Shorties</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7tdnbv95g5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1h8urb3</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Troll Vault</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8urb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1h8ubq6</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Accidentally matched my favorite hoodie</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ney9ypvyf5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1h8szih</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Xmas-birthday  season! 🎄 🔮 🎈 </t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71wsblplmf5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1h8smwl</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Help please.. now matter what I do my nails chip</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8smwl/help_please_now_matter_what_i_do_my_nails_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1h8rsdt</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh, so THIS is what ya’ll mean by “glow” </t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8rsdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1h8qv84</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying nail art 🎄 </t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8qv84</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1h8qq06</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Drink Me</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8qq06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1h8q30b</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Help Me Find This Colour Please!</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpd6ok87qe5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1h867hd</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Baby pink recs?</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo1kb8dzf95e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1h8i9vk</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Old Gooey Polish..is there a fix?</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1h8i9vk/old_gooey_polishis_there_a_fix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1h9du5w</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>A challenge</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9du5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1h9d6qk</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I name this set? </t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9d6qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1h9bchj</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Pink Animal Print Cherries</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jmux6tr3k5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1h9bb99</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Holiday Cinnamoroll Nails</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9bb99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1h9ang7</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready to see the Nutcracker ballet for the first time! </t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m83qpzcwj5e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1h98soo</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Been a while :)</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdcv2r2ldj5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1h97epi</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails by me 💚❤️ </t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxj2sai80j5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1h95utt</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Glam Christmas by me ✨🎄</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h95utt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1h92z24</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">throwback to my Halloween nails 🎃 </t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h92z24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1h92kat</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>feelin kinda icey! ❄️</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tmlvxu0uh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1h9172y</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>A set for a friend</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h9172y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1h90yhe</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>never stop what people will say always look for your own style</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h90yhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1h90w7j</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Pink Christmas is such a vibe!!!!!</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07lqqtd7gh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1h90li5</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>I made my own nails</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqxwxviudh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1h90jnd</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>if you want to be the queen of the Nile</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xi0ewf5dh5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1h90bvy</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Xander as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h90bvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1h908r0</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Princess Mononoke Press on practice </t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jni7b4yah5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1h8zju1</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>North Pole Chic</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xcvit7e5h5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1h8y809</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Holiday Nail Set 😍</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0foaczsuug5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1h8wgmo</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Simple Christmas nail art</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8wgmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1h8vye6</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>❄️ Winter Wonderland Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qhnt78kcg5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1h8uxqe</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Vintage jewelry inspired Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tc1rpynw3g5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1h8ublj</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>spooky nails 😋</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8ublj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1h8u18w</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>New set of christmas press ons</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8u18w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1h8t3ss</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Tortoise shell nails</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcunfpgpnf5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1h8sxyx</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gabriela Rodriguez </t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re1waat6mf5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1h8refi</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun cats eye and Christmas lights I did on my friend at work </t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndcvwvie6f5e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1h8oqmu</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Honest opinions on progress</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1h8oqmu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>